<commit_message>
Changed project name to S3
</commit_message>
<xml_diff>
--- a/Data/Config Prod.xlsx
+++ b/Data/Config Prod.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TVLK\Sprint 3\Traveloka_DataAutomation_Dispatcher_Email_S3\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D2C30B-948F-4405-9ECD-6CFEAA9EF30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D3C2DA-E041-4226-933E-E0D1BAD28D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -201,9 +201,6 @@
     <t>RPA_Moon_SenderName</t>
   </si>
   <si>
-    <t>RPA_Moon_Email_S2</t>
-  </si>
-  <si>
     <t>SheetIdConfigAccommodation</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>RPA_Moon_SheetIdConfig_Transport</t>
+  </si>
+  <si>
+    <t>RPA_Moon_Email_S3</t>
   </si>
 </sst>
 </file>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -643,7 +643,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -2851,7 +2851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2941,18 +2941,18 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
BP Javamifi splitted into 2 BPs Pocket & Esim
</commit_message>
<xml_diff>
--- a/Data/Config Prod.xlsx
+++ b/Data/Config Prod.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TVLK\Sprint 3\Traveloka_DataAutomation_Dispatcher_Email_S3\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D3C2DA-E041-4226-933E-E0D1BAD28D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6EBF68-3803-40E1-9457-E15A042E6CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>RPA_Moon_Email_S3</t>
+  </si>
+  <si>
+    <t>SheetIdConfigInterCon</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_SheetIdConfig_InterCon</t>
   </si>
 </sst>
 </file>
@@ -592,16 +598,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="74.88671875" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -649,7 +655,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -659,7 +665,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -670,7 +676,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="34.950000000000003" customHeight="1">
+    <row r="6" spans="1:26" ht="34.9" customHeight="1">
       <c r="B6" s="5"/>
       <c r="C6" s="3" t="s">
         <v>48</v>
@@ -1692,12 +1698,12 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1734,7 +1740,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1745,7 +1751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1859,7 +1865,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2851,16 +2857,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2955,7 +2961,14 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Update asset name for SheedId_IC
</commit_message>
<xml_diff>
--- a/Data/Config Prod.xlsx
+++ b/Data/Config Prod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TVLK\Sprint 3\Traveloka_DataAutomation_Dispatcher_Email_S3\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6EBF68-3803-40E1-9457-E15A042E6CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD9AE33-C08D-42AA-8D47-01F2A3AC33DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -219,7 +219,7 @@
     <t>SheetIdConfigInterCon</t>
   </si>
   <si>
-    <t>[Dev] RPA_Moon_SheetIdConfig_InterCon</t>
+    <t>RPA_Moon_SheetIdConfig_IC</t>
   </si>
 </sst>
 </file>
@@ -602,12 +602,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="74.85546875" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="2" max="2" width="74.88671875" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -655,7 +655,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -665,7 +665,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -676,7 +676,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="34.9" customHeight="1">
+    <row r="6" spans="1:26" ht="34.950000000000003" customHeight="1">
       <c r="B6" s="5"/>
       <c r="C6" s="3" t="s">
         <v>48</v>
@@ -1698,12 +1698,12 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1740,7 +1740,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1865,7 +1865,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2858,15 +2858,15 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>